<commit_message>
lagt til ny data i excelfil
</commit_message>
<xml_diff>
--- a/skostr_hoyde.xlsx
+++ b/skostr_hoyde.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\2025 ISTx100y Statistikk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/martilol_ntnu_no/Documents/3. semester/ISTG1002 - statistikk/Forprosjekt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB813E9D-D7B9-4DEE-910E-3DBF30FDB765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{FB813E9D-D7B9-4DEE-910E-3DBF30FDB765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6ECA566A-2775-4E1F-8FEB-7F7A9F5CDFFE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{17AD7C0B-BD46-864B-A286-7DB13EBD5FC9}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15240" xr2:uid="{17AD7C0B-BD46-864B-A286-7DB13EBD5FC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,9 +97,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013–2022">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -137,7 +137,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013–2022">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -243,7 +243,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013–2022">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -393,15 +393,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A645C9-12C5-5C40-AEE3-FEEA757065DC}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,7 +409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>40</v>
       </c>
@@ -417,7 +417,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>39</v>
       </c>
@@ -425,7 +425,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>45</v>
       </c>
@@ -433,7 +433,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>42</v>
       </c>
@@ -441,12 +441,20 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>38</v>
       </c>
       <c r="B6">
         <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>43</v>
+      </c>
+      <c r="B7">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>